<commit_message>
first version of report rmd
</commit_message>
<xml_diff>
--- a/outputs/summary_table.xlsx
+++ b/outputs/summary_table.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Scenario</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cumulative deaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deaths SD</t>
   </si>
   <si>
     <t xml:space="preserve">Base</t>
@@ -407,83 +410,95 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>43960</v>
+        <v>43961</v>
       </c>
       <c r="C2" t="n">
-        <v>639</v>
+        <v>631</v>
       </c>
       <c r="D2" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>43964</v>
       </c>
       <c r="F2" t="n">
-        <v>862</v>
+        <v>877</v>
       </c>
       <c r="G2" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H2" t="n">
-        <v>1324</v>
+        <v>1312</v>
+      </c>
+      <c r="I2" t="n">
+        <v>288</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>43957</v>
+        <v>43958</v>
       </c>
       <c r="C3" t="n">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D3" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>43963</v>
+        <v>43962</v>
       </c>
       <c r="F3" t="n">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="G3" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H3" t="n">
-        <v>1491</v>
+        <v>1474</v>
+      </c>
+      <c r="I3" t="n">
+        <v>327</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>43974</v>
       </c>
       <c r="C4" t="n">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="D4" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="F4" t="n">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="G4" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H4" t="n">
-        <v>1439</v>
+        <v>1450</v>
+      </c>
+      <c r="I4" t="n">
+        <v>357</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor corrections to report rmd
</commit_message>
<xml_diff>
--- a/outputs/summary_table.xlsx
+++ b/outputs/summary_table.xlsx
@@ -422,16 +422,16 @@
         <v>43961</v>
       </c>
       <c r="C2" t="n">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D2" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>43964</v>
+        <v>43965</v>
       </c>
       <c r="F2" t="n">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="G2" t="n">
         <v>22</v>
@@ -440,7 +440,7 @@
         <v>1312</v>
       </c>
       <c r="I2" t="n">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3">
@@ -451,25 +451,25 @@
         <v>43958</v>
       </c>
       <c r="C3" t="n">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D3" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>43962</v>
       </c>
       <c r="F3" t="n">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G3" t="n">
         <v>23</v>
       </c>
       <c r="H3" t="n">
-        <v>1474</v>
+        <v>1480</v>
       </c>
       <c r="I3" t="n">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4">
@@ -480,25 +480,25 @@
         <v>43974</v>
       </c>
       <c r="C4" t="n">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D4" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>43978</v>
       </c>
       <c r="F4" t="n">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="G4" t="n">
         <v>21</v>
       </c>
       <c r="H4" t="n">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="I4" t="n">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
flexible table_multi function, minor changes to report rmd
</commit_message>
<xml_diff>
--- a/outputs/summary_table.xlsx
+++ b/outputs/summary_table.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Scenario</t>
   </si>
@@ -41,13 +41,22 @@
     <t xml:space="preserve">Deaths SD</t>
   </si>
   <si>
-    <t xml:space="preserve">Base</t>
+    <t xml:space="preserve">Base (0%)</t>
   </si>
   <si>
     <t xml:space="preserve">20% reduction</t>
   </si>
   <si>
+    <t xml:space="preserve">40% reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50% reduction</t>
+  </si>
+  <si>
     <t xml:space="preserve">60% reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73% reduction</t>
   </si>
 </sst>
 </file>
@@ -419,28 +428,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>43961</v>
+        <v>43956</v>
       </c>
       <c r="C2" t="n">
-        <v>630</v>
+        <v>1489</v>
       </c>
       <c r="D2" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>43965</v>
+        <v>43962</v>
       </c>
       <c r="F2" t="n">
-        <v>878</v>
+        <v>1567</v>
       </c>
       <c r="G2" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="H2" t="n">
-        <v>1312</v>
+        <v>3018</v>
       </c>
       <c r="I2" t="n">
-        <v>286</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3">
@@ -451,25 +460,25 @@
         <v>43958</v>
       </c>
       <c r="C3" t="n">
-        <v>647</v>
+        <v>1451</v>
       </c>
       <c r="D3" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>43962</v>
+        <v>43963</v>
       </c>
       <c r="F3" t="n">
-        <v>910</v>
+        <v>1534</v>
       </c>
       <c r="G3" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H3" t="n">
-        <v>1480</v>
+        <v>3010</v>
       </c>
       <c r="I3" t="n">
-        <v>322</v>
+        <v>469</v>
       </c>
     </row>
     <row r="4">
@@ -477,28 +486,115 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="n">
+        <v>43958</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1459</v>
+      </c>
+      <c r="D4" t="n">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>43963</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1542</v>
+      </c>
+      <c r="G4" t="n">
+        <v>32</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3011</v>
+      </c>
+      <c r="I4" t="n">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>43966</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1259</v>
+      </c>
+      <c r="D5" t="n">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>43971</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1358</v>
+      </c>
+      <c r="G5" t="n">
+        <v>29</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2993</v>
+      </c>
+      <c r="I5" t="n">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>43974</v>
       </c>
-      <c r="C4" t="n">
-        <v>495</v>
-      </c>
-      <c r="D4" t="n">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>43978</v>
-      </c>
-      <c r="F4" t="n">
-        <v>718</v>
-      </c>
-      <c r="G4" t="n">
-        <v>21</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1449</v>
-      </c>
-      <c r="I4" t="n">
-        <v>360</v>
+      <c r="C6" t="n">
+        <v>1110</v>
+      </c>
+      <c r="D6" t="n">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>43979</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1211</v>
+      </c>
+      <c r="G6" t="n">
+        <v>29</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2962</v>
+      </c>
+      <c r="I6" t="n">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>43988</v>
+      </c>
+      <c r="C7" t="n">
+        <v>835</v>
+      </c>
+      <c r="D7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>43993</v>
+      </c>
+      <c r="F7" t="n">
+        <v>932</v>
+      </c>
+      <c r="G7" t="n">
+        <v>25</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2879</v>
+      </c>
+      <c r="I7" t="n">
+        <v>597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct LoS, include ward beds output in report tables
</commit_message>
<xml_diff>
--- a/outputs/summary_table.xlsx
+++ b/outputs/summary_table.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Scenario</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t xml:space="preserve">HDU SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak ward bed needs timing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean peak ward bed needs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ward SD</t>
   </si>
   <si>
     <t xml:space="preserve">Cumulative deaths</t>
@@ -422,179 +431,242 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>43956</v>
+        <v>43958</v>
       </c>
       <c r="C2" t="n">
-        <v>1489</v>
+        <v>1807</v>
       </c>
       <c r="D2" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>43962</v>
+        <v>43964</v>
       </c>
       <c r="F2" t="n">
-        <v>1567</v>
+        <v>978</v>
       </c>
       <c r="G2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H2" t="n">
-        <v>3018</v>
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>43976</v>
       </c>
       <c r="I2" t="n">
-        <v>463</v>
+        <v>1439</v>
+      </c>
+      <c r="J2" t="n">
+        <v>33</v>
+      </c>
+      <c r="K2" t="n">
+        <v>3012</v>
+      </c>
+      <c r="L2" t="n">
+        <v>473</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="C3" t="n">
-        <v>1451</v>
+        <v>1766</v>
       </c>
       <c r="D3" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>43963</v>
+        <v>43966</v>
       </c>
       <c r="F3" t="n">
-        <v>1534</v>
+        <v>959</v>
       </c>
       <c r="G3" t="n">
-        <v>30</v>
-      </c>
-      <c r="H3" t="n">
-        <v>3010</v>
+        <v>27</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>43977</v>
       </c>
       <c r="I3" t="n">
-        <v>469</v>
+        <v>1417</v>
+      </c>
+      <c r="J3" t="n">
+        <v>32</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3011</v>
+      </c>
+      <c r="L3" t="n">
+        <v>476</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>43958</v>
+        <v>43960</v>
       </c>
       <c r="C4" t="n">
-        <v>1459</v>
+        <v>1773</v>
       </c>
       <c r="D4" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>43963</v>
+        <v>43965</v>
       </c>
       <c r="F4" t="n">
-        <v>1542</v>
+        <v>962</v>
       </c>
       <c r="G4" t="n">
-        <v>32</v>
-      </c>
-      <c r="H4" t="n">
-        <v>3011</v>
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>43977</v>
       </c>
       <c r="I4" t="n">
-        <v>468</v>
+        <v>1420</v>
+      </c>
+      <c r="J4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K4" t="n">
+        <v>3010</v>
+      </c>
+      <c r="L4" t="n">
+        <v>478</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43966</v>
+        <v>43968</v>
       </c>
       <c r="C5" t="n">
-        <v>1259</v>
+        <v>1548</v>
       </c>
       <c r="D5" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>43971</v>
+        <v>43973</v>
       </c>
       <c r="F5" t="n">
-        <v>1358</v>
+        <v>868</v>
       </c>
       <c r="G5" t="n">
-        <v>29</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2993</v>
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>43985</v>
       </c>
       <c r="I5" t="n">
-        <v>503</v>
+        <v>1291</v>
+      </c>
+      <c r="J5" t="n">
+        <v>32</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2992</v>
+      </c>
+      <c r="L5" t="n">
+        <v>511</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>43974</v>
+        <v>43975</v>
       </c>
       <c r="C6" t="n">
-        <v>1110</v>
+        <v>1375</v>
       </c>
       <c r="D6" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>43979</v>
+        <v>43981</v>
       </c>
       <c r="F6" t="n">
-        <v>1211</v>
+        <v>788</v>
       </c>
       <c r="G6" t="n">
-        <v>29</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2962</v>
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>43993</v>
       </c>
       <c r="I6" t="n">
-        <v>522</v>
+        <v>1181</v>
+      </c>
+      <c r="J6" t="n">
+        <v>32</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2959</v>
+      </c>
+      <c r="L6" t="n">
+        <v>531</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>43988</v>
+        <v>43990</v>
       </c>
       <c r="C7" t="n">
-        <v>835</v>
+        <v>1047</v>
       </c>
       <c r="D7" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="F7" t="n">
-        <v>932</v>
+        <v>621</v>
       </c>
       <c r="G7" t="n">
-        <v>25</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2879</v>
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>44007</v>
       </c>
       <c r="I7" t="n">
-        <v>597</v>
+        <v>947</v>
+      </c>
+      <c r="J7" t="n">
+        <v>28</v>
+      </c>
+      <c r="K7" t="n">
+        <v>2880</v>
+      </c>
+      <c r="L7" t="n">
+        <v>602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>